<commit_message>
Added S.marinoi size to diatom timeseries. Looking at relationship between abundance and Tchla.
</commit_message>
<xml_diff>
--- a/files/s_mar_size.xlsx
+++ b/files/s_mar_size.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justin.belluz\Documents\R\calvert_spatial\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0F6A5A-B6AA-4C00-936F-76B6E63936D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF7207B-F41E-45FA-9A21-97A5BEFDB982}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="14604" xr2:uid="{536A1E6A-78FF-43E7-90E2-88BF2FE3DC0C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>CPHY476</t>
   </si>
@@ -217,13 +217,88 @@
   </si>
   <si>
     <t>species</t>
+  </si>
+  <si>
+    <t>CPHY528</t>
+  </si>
+  <si>
+    <t>CPHY531</t>
+  </si>
+  <si>
+    <t>CPHY533</t>
+  </si>
+  <si>
+    <t>CPHY478</t>
+  </si>
+  <si>
+    <t>CPHY485</t>
+  </si>
+  <si>
+    <t>CPHY489</t>
+  </si>
+  <si>
+    <t>CPHY492</t>
+  </si>
+  <si>
+    <t>CPHY486</t>
+  </si>
+  <si>
+    <t>CPHY499</t>
+  </si>
+  <si>
+    <t>CPHY502</t>
+  </si>
+  <si>
+    <t>CPHY508</t>
+  </si>
+  <si>
+    <t>CPHY512</t>
+  </si>
+  <si>
+    <t>CPHY513</t>
+  </si>
+  <si>
+    <t>CPHY517</t>
+  </si>
+  <si>
+    <t>CPHY520</t>
+  </si>
+  <si>
+    <t>CPHY497</t>
+  </si>
+  <si>
+    <t>CPHY403</t>
+  </si>
+  <si>
+    <t>CPHY408</t>
+  </si>
+  <si>
+    <t>CPHY423</t>
+  </si>
+  <si>
+    <t>CPHY432</t>
+  </si>
+  <si>
+    <t>CPHY445</t>
+  </si>
+  <si>
+    <t>CPHY451</t>
+  </si>
+  <si>
+    <t>CPHY457</t>
+  </si>
+  <si>
+    <t>CPHY462</t>
+  </si>
+  <si>
+    <t>CPHY470</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,13 +320,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -263,21 +350,74 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -718,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71159C60-B509-4292-9C73-672B96F975D6}">
-  <dimension ref="A1:BJ3"/>
+  <dimension ref="A1:CI3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="BZ5" sqref="BZ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -729,7 +869,7 @@
     <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -916,8 +1056,83 @@
       <c r="BJ1" t="s">
         <v>60</v>
       </c>
+      <c r="BK1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BO1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="BP1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="BQ1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BZ1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>80</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>81</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>82</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>83</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>84</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>85</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>86</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>87</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>88</v>
+      </c>
     </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>61</v>
       </c>
@@ -1104,8 +1319,83 @@
       <c r="BJ2">
         <v>446000</v>
       </c>
+      <c r="BK2" s="6">
+        <v>54736</v>
+      </c>
+      <c r="BL2" s="6">
+        <v>1092000</v>
+      </c>
+      <c r="BM2" s="6">
+        <v>98864</v>
+      </c>
+      <c r="BN2" s="3">
+        <v>0</v>
+      </c>
+      <c r="BO2" s="1">
+        <v>320</v>
+      </c>
+      <c r="BP2" s="1">
+        <v>21888</v>
+      </c>
+      <c r="BQ2">
+        <v>140000</v>
+      </c>
+      <c r="BR2">
+        <v>121360</v>
+      </c>
+      <c r="BS2">
+        <v>820000</v>
+      </c>
+      <c r="BT2">
+        <v>446000</v>
+      </c>
+      <c r="BU2">
+        <v>0</v>
+      </c>
+      <c r="BV2">
+        <v>79927</v>
+      </c>
+      <c r="BW2">
+        <v>80</v>
+      </c>
+      <c r="BX2">
+        <v>160</v>
+      </c>
+      <c r="BY2">
+        <v>400</v>
+      </c>
+      <c r="BZ2">
+        <v>125000</v>
+      </c>
+      <c r="CA2">
+        <v>2960</v>
+      </c>
+      <c r="CB2">
+        <v>0</v>
+      </c>
+      <c r="CC2">
+        <v>406000</v>
+      </c>
+      <c r="CD2">
+        <v>57224</v>
+      </c>
+      <c r="CE2">
+        <v>339966</v>
+      </c>
+      <c r="CF2">
+        <v>20600</v>
+      </c>
+      <c r="CG2">
+        <v>219000</v>
+      </c>
+      <c r="CH2">
+        <v>334000</v>
+      </c>
+      <c r="CI2">
+        <v>78736</v>
+      </c>
     </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:87" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>62</v>
       </c>
@@ -1291,46 +1581,136 @@
       </c>
       <c r="BJ3">
         <v>71841</v>
+      </c>
+      <c r="BK3" s="6">
+        <v>18864</v>
+      </c>
+      <c r="BL3" s="6">
+        <v>394000</v>
+      </c>
+      <c r="BM3" s="6">
+        <v>81104</v>
+      </c>
+      <c r="BN3" s="1">
+        <v>1960</v>
+      </c>
+      <c r="BO3" s="1">
+        <v>89984</v>
+      </c>
+      <c r="BP3" s="1">
+        <v>71841</v>
+      </c>
+      <c r="BQ3">
+        <v>9102</v>
+      </c>
+      <c r="BR3">
+        <v>50693</v>
+      </c>
+      <c r="BS3">
+        <v>20800</v>
+      </c>
+      <c r="BT3">
+        <v>660000</v>
+      </c>
+      <c r="BU3">
+        <v>72816</v>
+      </c>
+      <c r="BV3">
+        <v>974000</v>
+      </c>
+      <c r="BW3">
+        <v>4000</v>
+      </c>
+      <c r="BX3">
+        <v>6048</v>
+      </c>
+      <c r="BY3">
+        <v>7502</v>
+      </c>
+      <c r="BZ3">
+        <v>304000</v>
+      </c>
+      <c r="CA3">
+        <v>0</v>
+      </c>
+      <c r="CB3">
+        <v>280</v>
+      </c>
+      <c r="CC3">
+        <v>3312</v>
+      </c>
+      <c r="CD3">
+        <v>124320</v>
+      </c>
+      <c r="CE3">
+        <v>7344</v>
+      </c>
+      <c r="CF3">
+        <v>1836</v>
+      </c>
+      <c r="CG3">
+        <v>6764</v>
+      </c>
+      <c r="CH3">
+        <v>3330</v>
+      </c>
+      <c r="CI3">
+        <v>4366</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1">
+    <cfRule type="duplicateValues" dxfId="17" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V1">
+    <cfRule type="duplicateValues" dxfId="16" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W1">
+    <cfRule type="duplicateValues" dxfId="15" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y1">
+    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z1">
+    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA1">
     <cfRule type="duplicateValues" dxfId="12" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V1">
+  <conditionalFormatting sqref="AB1">
     <cfRule type="duplicateValues" dxfId="11" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W1">
+  <conditionalFormatting sqref="AD1">
     <cfRule type="duplicateValues" dxfId="10" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y1">
+  <conditionalFormatting sqref="AE1">
     <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z1">
+  <conditionalFormatting sqref="AF1">
     <cfRule type="duplicateValues" dxfId="8" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA1">
+  <conditionalFormatting sqref="AG1">
     <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB1">
+  <conditionalFormatting sqref="AI1">
     <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD1">
+  <conditionalFormatting sqref="AK1">
     <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE1">
+  <conditionalFormatting sqref="BN1">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF1">
+  <conditionalFormatting sqref="BO1">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG1">
+  <conditionalFormatting sqref="BP1">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI1">
+  <conditionalFormatting sqref="BQ1">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK1">
+  <conditionalFormatting sqref="BR1">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>